<commit_message>
Added comments to template
</commit_message>
<xml_diff>
--- a/IEC62559-2_TEMPLATE.xlsx
+++ b/IEC62559-2_TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Arse\nntt\Proyectos\H2020\ENERGY\BRIDGE\USE CASE REPOSITORY\TO TEST THE TOOL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trabajo\BRIDGE\DOCS\UC-repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67608985-6CD8-4200-8890-D63C4869FA1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDAC8F29-EF5C-4CA5-9D6F-4D430B664FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IEC62559-2" sheetId="1" r:id="rId1"/>
@@ -25,8 +25,1345 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Lucas Pons Bayarri</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{E23633B1-EBB7-4C89-A0C2-55A29391A52C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use cases can be used in various areas (e.g. energy system). Within these areas, different domains are used to define/determine a more specific subgrouping. Zones might describe additional zones with an automation system or a reference architecture (SGAM). Experts in a particular field could suggest their set of domain (and zones) in order to provide a common understanding how to group use cases within a complex area. These predefined domains (and zones) can be chosen by the author of the use case (preselection). The author can select one or more domains and zone, comma separated, as  it is usual that use cases are crossing different domains and zones. Example domains: Generation, transmission, DER, distribution, customer premises. Example zones: Process, field, station, operation, enterprise, market</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{76F9918A-7218-4FC4-B48E-D79D203DBCCC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per version. Do not remove previous columns in order to keep track of past versions. These set of field will be expanded in columns on any new version</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{EF0BF706-2A10-43B3-A25A-DCA2DFF030A9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Comma-separated list</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0" shapeId="0" xr:uid="{5DB4FE69-7B66-4AAB-B160-A0B2AAADB820}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+will be used within the standardization organizations. The procedures for validation of use cases or actors will be defined in part 1 of this standard.
+EXAMPLE Similar to working draft, committee draft (CD) for comments, committee draft for vote (CDV), for voting (similar FDIS), final</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B16" authorId="0" shapeId="0" xr:uid="{6E903193-5FCC-429C-9B92-A34C145579FB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Comma separated list of related use cases</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{5DF745C5-06D5-4560-9851-53A5036C3981}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per KPI. This set of columns will expand in columns on any addtional KPI
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="0" shapeId="0" xr:uid="{9D68FB42-2D66-4D2F-9B3F-C1379220118A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert as much assumptions and prerequisites as needed in columns. This set of rows will be expanded in columns</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B29" authorId="0" shapeId="0" xr:uid="{0AFAD6EB-8359-4129-985E-79591C15FD2C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Known relations to other use cases can be provided here if e.g.
+the use case is a more detailed one related to a high level use case, or it is an alternative to an
+existing use case. The type of relation like “include”, “extends”, “invokes” might be used in
+order to specify this relation in more detail.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B30" authorId="0" shapeId="0" xr:uid="{F8879508-9B29-4810-919F-545C7B865FFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Use cases can be described on different levels (refer to IEC62559-1 for
+examples). Currently there is no fixed hierarchy for use cases defined, but some most common
+examples are provided.
+EXAMPLE High level use case, generic use case, specialised use cases.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B31" authorId="0" shapeId="0" xr:uid="{087376AA-D4CD-47FB-B92F-6B2CA21863D3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+EXAMPLE: Obligatory/mandatory, optional, nice to have.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B32" authorId="0" shapeId="0" xr:uid="{B2AACC68-2DC9-4EBF-B8DA-565EA1BE23A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+On international level, the use case description might be
+generic enough to describe a use case in a more general way independently from the national
+or regional market design. But use cases might be used to describe regional or national
+specific circumstances like laws or even project-specific details. If the use case reflects those
+circumstances, it should be characterized accordingly.
+EXAMPLE National, "Country".</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B33" authorId="0" shapeId="0" xr:uid="{6DB65455-BD2B-4172-A822-27973131984E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This field can help to classify the main focus of the use case.
+EXAMPLE Technical/system use case, business use cases (e.g. market processes), political, test use cases.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B35" authorId="0" shapeId="0" xr:uid="{4CB07AED-B3D4-45CF-9C6B-F372D1E4B11B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one row per general remark of the use case. This row will be expanded  by columns
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B36" authorId="0" shapeId="0" xr:uid="{FAD85E48-4A7F-4012-B859-B38901F11689}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+for further comments which are not considered elsewhere.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B37" authorId="0" shapeId="0" xr:uid="{AF6FAAE1-ED2E-45A5-A641-E4A8C5471417}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per diagram associated to this use case. This set of rows will be expanded by columns.
+Each diagram should be later uploaded to the github along with this template filled up. The name of the diagram files uploaded must match thr name specified in this section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B39" authorId="0" shapeId="0" xr:uid="{58C3722C-A687-4F37-A103-859ADA17A38C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Activity, component, functional, sequence, etc..</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B40" authorId="0" shapeId="0" xr:uid="{7A596E70-3A3A-4A8E-AA94-0524988F3921}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+image or URL</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B41" authorId="0" shapeId="0" xr:uid="{405E3565-597D-459E-8938-67094151FE2B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert the name of the diagram exactly like the one that will be uploaded 
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B43" authorId="0" shapeId="0" xr:uid="{41C1E9B3-062B-4116-B180-B882BF5AF29B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per actor. These set of rows will be expanded by columns. 
+The concept of an “actor” is very general and can cover:
+People (their roles or jobs), systems, databases, organizations, and devices involved in or
+affected by the use case: e.g. operators, system administrators, technicians, end users,
+service personnel, executives, SCADA system, real-time database, regional transmission
+operator (RTO), remote terminal units (RTU), intelligent electronic devices (IED) and even the power system. It is recommended to use actors as described in the ENTSO-E role model: https://eepublicdownloads.entsoe.eu/clean-documents/EDI/Library/HRM/Harmonised_Role_Model_2020-01.pdf
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="0" shapeId="0" xr:uid="{DD8A39C2-5F38-4993-B36F-D5816CAD2DED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The actor list can be grouped in order to provide a better overview. Naming convention: For complex groupings, the group name can be “dot-delimited”. EXAMPLE (area.domain.) main.sub.subsub. The grouping may follow the suggested domains/zones previous section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B45" authorId="0" shapeId="0" xr:uid="{705A17E3-010C-4E4B-BC45-74443F9A69AD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Brief description of the group</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B46" authorId="0" shapeId="0" xr:uid="{C7A6BEF6-45FF-4EC9-83B2-3CA2F62FF1AE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Actor name according to an existing taxonomy OR actor name especifically defined for this project
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="0" shapeId="0" xr:uid="{A938614F-574C-4CB6-B01B-D1F721268827}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+If the actor is already defined in an existing and well-know actors taxonomy, just add here the name of the taxonomy (EXAMPLE: ENTSO-E role model). If not, here the type of actor should be provided </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B48" authorId="0" shapeId="0" xr:uid="{47F7770E-DCAF-4866-AA18-DB4FD6134157}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In case the actor is not described in any existing taxonomy, the description mandatory. If the actor is already described ina taxonomy and the taxonomy is specified in the previos field, this field is not required</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B50" authorId="0" shapeId="0" xr:uid="{C06302B3-FA12-46CA-91F2-FD3183970606}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per reference. These set of rows will be expanded by columns.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B53" authorId="0" shapeId="0" xr:uid="{80FC2948-832E-4FF3-B439-3B0BCBE1921D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+There are different reference types as shown in the examples above (e.g.
+standards, regulation, contract, others like publications)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B54" authorId="0" shapeId="0" xr:uid="{27F575A1-754A-4BE2-84BC-080D51EF939A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Any references shall be identified that might restrict or affect the design,
+understanding, and requirements of the use case, including contracts, regulations, policies,
+financial considerations, engineering constraints, pollution constraints, and other environmental
+quality issues</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B55" authorId="0" shapeId="0" xr:uid="{20ACBDE2-E5D7-4E5B-BC29-C547F9AA5EEA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+e.g. NP, CD, CDV, FDIS, IS</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B56" authorId="0" shapeId="0" xr:uid="{88F7339A-57EE-4F2F-8830-8C51BBA0D22B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Where does the document influence the use case? e.g. copy
+right, IPR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B57" authorId="0" shapeId="0" xr:uid="{7BC926E6-471B-4CC3-B62D-BE93D8DEF92D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Who published the document?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B58" authorId="0" shapeId="0" xr:uid="{250BF442-3EBB-40D3-BFE8-9425C8BADFDB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+If available, a public link can be provided (e.g. to the IEC webstore for standards).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B60" authorId="0" shapeId="0" xr:uid="{3E8790EC-056D-472F-9525-CAC317DC54A8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Focuses on describing scenarios of the use case with a step-step analysis
+(sequence description).</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B61" authorId="0" shapeId="0" xr:uid="{9EA5D997-FFC4-426A-86F2-2D03BEF32265}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per condition. These set of rows will be expanded by columns</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B65" authorId="0" shapeId="0" xr:uid="{3C586E16-8124-415E-8155-0871AE3150BE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+describes which actor(s) trigger(s) this scenario.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B66" authorId="0" shapeId="0" xr:uid="{C594F556-49E6-4E31-A501-29D4D6C35356}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+describes which event(s) trigger(s) this scenario.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B67" authorId="0" shapeId="0" xr:uid="{035184D6-3907-48C5-B033-E21AB48F8A57}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Describes which condition(s) should have been met before this scenario
+happens.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B68" authorId="0" shapeId="0" xr:uid="{200593C5-8309-453D-8786-CE45FCCAB461}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+describes which condition(s) should prevail after this scenario happens The
+post conditions may also define “success” or “failure” conditions for each use case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B69" authorId="0" shapeId="0" xr:uid="{F0B33A69-30E8-43D7-AF26-CE3DF9B49169}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per step. These set of rows will be expanded by columns. 
+For the scenario, all the steps performed shall be described going from start to end using
+simple verbs like – get, put, cancel, subscribe etc. Steps shall be numbered sequentially – 1, 2, 3 and so on. 
+Should the scenario require detailed descriptions of steps that are also used by other use
+cases, it should be considered creating a new “sub” use case, then referring to that
+“subroutine” in this scenario. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B70" authorId="0" shapeId="0" xr:uid="{DFE4AF1F-9272-444B-B5E3-73640DAE125D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Refers to the name of one of the scenarios defined in the previous section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B72" authorId="0" shapeId="0" xr:uid="{5C3C6DAB-725A-4811-8FE2-0771E449C06D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+The event that triggers the step. This might be completion of the previous step. 
+EXAMPLE A human requesting the function, data being reported periodically, or a power system event</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B73" authorId="0" shapeId="0" xr:uid="{DB6AAFA8-8ADD-44D3-8B91-38BFA096E81F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Label that would appear in a process diagram. Action verbs should
+be used when naming activity.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B74" authorId="0" shapeId="0" xr:uid="{27314879-FFD5-4EC9-A7A4-61B2CA089550}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This describes what action takes place in this step. The focus
+should be less on the algorithms of the applications and more on the interactions and
+information flows between actors.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B75" authorId="0" shapeId="0" xr:uid="{332C013D-CD60-45A0-A997-3492CC6E6F03}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This column identifies the nature of the information flow and the originator of the
+information. Available options are CREATE, GET, CHANGE, DELETE, CANCEL, EXECUTE
+derived from IEC 61968-100:2013, 6.2.2. Additionally, REPORT, TIMER and REPEAT are
+suggested.
+CREATE means that an information object is to be created at the Producer.
+GET (this is the default value if none is populated) means that the Receiver requests
+information from the Producer (default).
+CHANGE means that information is to be updated. Producer updates the Receiver’s
+information.
+DELETE means that information is to be deleted. Producer deletes information from the
+Receiver.
+CANCEL, CLOSE imply actions related to processes, such as the closure of a work order or the cancellation of a control request.
+EXECUTE is used when a complex transaction is being conveyed using a service, which potentially contains more than one verb.
+REPORT is used to represent transferral of unsolicited information or asynchronous information flows. Producer provides information to the Receiver.
+TIMER is used to represent a waiting period. When using the TIMER service, the Information Producer and Information Receiver fields shall refer to the same actor.
+REPEAT is used to indicate that a series of steps is repeated until a condition or trigger event. The condition is specified as the text in the “Event” column for this row or step.
+Following the word REPEAT, shall appear, in parenthesis, the first and last step numbers of the series to be repeated in the following form REPEAT(X-Y) where X is the first step and Y is the last step.
+These common service definitions are related to automation/information or communication systems. In case the use case template is applied in other domains,
+further services might be used and described.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B76" authorId="0" shapeId="0" xr:uid="{7C9FA788-BEA6-4655-B8A9-E56EE11EE9D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This identifies the producer or source of the information. This should be one of the actors in the reference template section.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B77" authorId="0" shapeId="0" xr:uid="{FE444ED9-B19E-42F6-AE0C-07D1E83F79C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This identifies the receiver of the information. This should also be one of
+the actors identified above</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B78" authorId="0" shapeId="0" xr:uid="{9BCD2BAA-3C74-4F7D-9E81-9C90C222624F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+This describes briefly the information to be exchanged between the two actors – information producer and information receiver:
+– Input to the use case from some external sources that is not described in this use case.
+– Internal to the use case (e.g. between different applications and systems within the use
+case).
+– Output from the use case that will be used by other actors/entities not included in this
+use case.
+– This column should not contain technology issues/requirements.
+– It is allowed to list several information in one step, comma separated.
+– Summarizing the information exchanged between two actors based on the relevant set
+of use cases can characterize the needed communication/message payload.
+– Detailed information exchange should be identified using an ID (“Name of Information”).
+Such name should include the source namespace, if not referring to the by-default one.
+In this case, the column only contains the ID of the exchanged information which link to
+more details about the information in a separate table in the following template section 5
+which is used for all steps of the use case.
+Here the information can use a short ID referring to template section 5 for further details.
+Several information exchanged IDs can be listed, comma separated.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B79" authorId="0" shapeId="0" xr:uid="{A83FCF29-5C0A-4CC3-960F-F21422CC65D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Refers to the Number of one of the scenarios defined in the previous section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B80" authorId="0" shapeId="0" xr:uid="{F35EE014-07EF-41A9-893C-DD6378895777}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Insert one column per information item. These set of rows will be expanded by columns. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B81" authorId="0" shapeId="0" xr:uid="{B076B93E-72DC-481D-9EA4-DF891FA9D3E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+the requirement id Can be used to define requirements referring to the information and not to the step as in the step by step analysis (see template section 6 below):
+EXAMPLE Data protection class corresponding to this information object.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B82" authorId="0" shapeId="0" xr:uid="{6268A0E6-5252-4F5C-9998-4BDE0DD3F291}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unique ID which identifies the selected information in the context of the use case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B83" authorId="0" shapeId="0" xr:uid="{698116E6-BE26-4262-B9B2-B5175BD78E63}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unique ID which identifies the selected information in the context of the use case.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B84" authorId="0" shapeId="0" xr:uid="{A0649456-69CD-44E8-8526-0BE9EA17F135}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Lucas Pons Bayarri:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Brief description, in case a reference to existing data
+models/information classes should be added. Using existing canonical data models is recommended.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="85">
   <si>
     <t>1 Description of the use case</t>
   </si>
@@ -278,6 +1615,9 @@
   </si>
   <si>
     <t>Optional: The cells in blue are for multiple objects, that can be completed when needed.</t>
+  </si>
+  <si>
+    <t>Instructions are provided as comments in the rows</t>
   </si>
 </sst>
 </file>
@@ -287,7 +1627,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -372,6 +1712,39 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -540,7 +1913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -567,6 +1940,9 @@
     <xf numFmtId="164" fontId="0" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,10 +2325,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -966,6 +2344,9 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="24" t="s">
+        <v>84</v>
+      </c>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,18 +3060,17 @@
       <c r="E79" s="19"/>
       <c r="F79" s="19"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="12"/>
+    <row r="80" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="B80" s="6"/>
       <c r="C80" s="22"/>
       <c r="D80" s="22"/>
       <c r="E80" s="22"/>
       <c r="F80" s="22"/>
     </row>
-    <row r="81" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
-        <v>72</v>
-      </c>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B81" s="16" t="s">
         <v>73</v>
       </c>
@@ -1732,6 +3112,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fixed possble values image type and uri type
</commit_message>
<xml_diff>
--- a/IEC62559-2_TEMPLATE.xlsx
+++ b/IEC62559-2_TEMPLATE.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trabajo\BRIDGE\DOCS\UC-repository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\trabajo\BRIDGE\UC-repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDAC8F29-EF5C-4CA5-9D6F-4D430B664FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{57792D65-EE37-4919-9623-20E4DF321A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="27120" windowHeight="16440" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IEC62559-2" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Activity, component, functional, sequence, etc..</t>
+"domain_overview", "use_case_overview", "documentation", "scenarios_flowchart", "scenario_overview", "activities_flowchart", "activity_overview", "business_objects_overview", "role_model", "other" or nothing (default="other")</t>
         </r>
       </text>
     </comment>
@@ -452,7 +452,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-image or URL</t>
+"UMLDiagram", "image" or nothing</t>
         </r>
       </text>
     </comment>
@@ -1945,8 +1945,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2030,7 +2030,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2329,10 +2329,10 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
     <col min="2" max="2" width="56.42578125" customWidth="1"/>
@@ -3124,7 +3124,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="81" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>